<commit_message>
fix: Include DECODE column in CT validation for completeness
- Updated validate_ct_conformance to check coded_value, submission_value, AND decode
- Validation now properly matches raw data values against DECODE shorthand values
- Example: 'Possibly' → 'POSSIBLY' (from DECODE column), 'UNLIKELY' → 'UNLIKELY RELATED' (submission)
- Enables validation of codelists that use DECODE for user-friendly/short forms
</commit_message>
<xml_diff>
--- a/study-pilot/metadata/Study_CT.xlsx
+++ b/study-pilot/metadata/Study_CT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\OneDrive - Alma Mater Studiorum Università di Bologna\Desktop\Repo\sdtm-builder\study-pilot\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE84856-67A2-43BC-A4FA-51B11279093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F15C170-AFDA-4E8B-A17C-80DD6A90E968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2880" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19150,7 +19150,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="25.5" customHeight="1"/>
@@ -57093,15 +57093,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="2fdc3c6c-6d33-4619-8401-32a1eeb41279" xsi:nil="true"/>
@@ -57111,6 +57102,15 @@
     <_Flow_SignoffStatus xmlns="4acd8c21-52dc-4e0a-ba78-2d26a7f06ee1" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57133,14 +57133,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7661C9F-2AC3-4F9D-B3CB-F4540758D4DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{140AEEBC-EC54-4AD1-84C7-3F36B88F9A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -57157,6 +57149,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7661C9F-2AC3-4F9D-B3CB-F4540758D4DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4720ed5e-c545-46eb-99a5-958dd333e9f2}" enabled="0" method="" siteId="{4720ed5e-c545-46eb-99a5-958dd333e9f2}" removed="1"/>

</xml_diff>

<commit_message>
feat: Add auto KEYS-based SEQ derivation for domain sequence variables
- Implement automatic sequence number derivation using KEYS metadata
- Derives SEQ (e.g., AESEQ, EXSEQ) based on grouping and sorting KEYS
- Properly handles null KEYS and sorting KEYS as independent sequences
- Validates grouping by KEYS to ensure proper sequencing
- No breaking changes to existing API

Closes: Auto-derivation for domain sequence variables
</commit_message>
<xml_diff>
--- a/study-pilot/metadata/Study_CT.xlsx
+++ b/study-pilot/metadata/Study_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\OneDrive - Alma Mater Studiorum Università di Bologna\Desktop\Repo\sdtm-builder\study-pilot\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F15C170-AFDA-4E8B-A17C-80DD6A90E968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18B895B-D84E-48FC-9689-A33D9E742E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2880" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28785" yWindow="3015" windowWidth="21585" windowHeight="13665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codelists" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11481" uniqueCount="3001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11481" uniqueCount="3000">
   <si>
     <t>Select</t>
   </si>
@@ -9041,9 +9041,6 @@
   </si>
   <si>
     <t>PROBABLY</t>
-  </si>
-  <si>
-    <t>UNLIKELY</t>
   </si>
 </sst>
 </file>
@@ -19148,9 +19145,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G2155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="25.5" customHeight="1"/>
@@ -19555,7 +19552,9 @@
       <c r="E23" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>1731</v>
+      </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="25.5" customHeight="1">
@@ -19571,9 +19570,6 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
         <v>735</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>3000</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -57093,6 +57089,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="2fdc3c6c-6d33-4619-8401-32a1eeb41279" xsi:nil="true"/>
@@ -57102,15 +57107,6 @@
     <_Flow_SignoffStatus xmlns="4acd8c21-52dc-4e0a-ba78-2d26a7f06ee1" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57133,6 +57129,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7661C9F-2AC3-4F9D-B3CB-F4540758D4DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{140AEEBC-EC54-4AD1-84C7-3F36B88F9A9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -57149,14 +57153,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7661C9F-2AC3-4F9D-B3CB-F4540758D4DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4720ed5e-c545-46eb-99a5-958dd333e9f2}" enabled="0" method="" siteId="{4720ed5e-c545-46eb-99a5-958dd333e9f2}" removed="1"/>

</xml_diff>